<commit_message>
PI controller update and fixes
Major:
• all PI controllers with Back-calculation replaced with PI controllers with Clamping to reduce the number of parameters and simplify calculations

Minor:
• fixed the ADC calibration for potetiometer input when ADCx_MIN > 0
• fixed bug: small shock at initialization when current limit I_MOT_MAX is set very small e.g. 1 A
</commit_message>
<xml_diff>
--- a/01_Matlab/03_CreateParamTable/tableParamType.xlsx
+++ b/01_Matlab/03_CreateParamTable/tableParamType.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18525" yWindow="0" windowWidth="17280" windowHeight="8640" activeTab="1"/>
+    <workbookView xWindow="21450" yWindow="0" windowWidth="17280" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="87">
   <si>
     <t>Parameter</t>
   </si>
@@ -64,27 +64,18 @@
     <t>cf_iqKiLimProt</t>
   </si>
   <si>
-    <t>cf_nKb</t>
-  </si>
-  <si>
     <t>cf_nKi</t>
   </si>
   <si>
     <t>cf_nKp</t>
   </si>
   <si>
-    <t>cf_iqKb</t>
-  </si>
-  <si>
     <t>cf_iqKi</t>
   </si>
   <si>
     <t>cf_iqKp</t>
   </si>
   <si>
-    <t>cf_idKb</t>
-  </si>
-  <si>
     <t>cf_idKi</t>
   </si>
   <si>
@@ -184,12 +175,6 @@
     <t>Current filter coefficient</t>
   </si>
   <si>
-    <t>D axis back calculation gain for integral anti-windup</t>
-  </si>
-  <si>
-    <t>Q axis back calculation gain for integral anti-windup</t>
-  </si>
-  <si>
     <t>D axis current control I gain</t>
   </si>
   <si>
@@ -212,9 +197,6 @@
   </si>
   <si>
     <t>Speed control I gain</t>
-  </si>
-  <si>
-    <t>Speed control back calculation gain for integral anti-windup</t>
   </si>
   <si>
     <t>Speed limit protection gain (only used in VLT_MODE and TRQ_MODE)</t>
@@ -399,8 +381,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:D43" totalsRowShown="0">
-  <autoFilter ref="B3:D43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:D40" totalsRowShown="0">
+  <autoFilter ref="B3:D40"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Parameter"/>
     <tableColumn id="2" name="DataType"/>
@@ -673,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B41"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,319 +680,295 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1020,10 +978,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D43"/>
+  <dimension ref="B3:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,10 +998,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1051,117 +1009,117 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -1169,321 +1127,288 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" t="s">
-        <v>90</v>
+        <v>26</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>71</v>
+      <c r="B35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sinusoidal Control Type
Sinusoidal Control Type is now available is this branch. To select it go in config.h and change CTRL_TYP_SEL to 1. By default FOC control type is selcted.
Note: SPEED and TORQUE modes are not available for Sinusoidal control type.
</commit_message>
<xml_diff>
--- a/01_Matlab/03_CreateParamTable/tableParamType.xlsx
+++ b/01_Matlab/03_CreateParamTable/tableParamType.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22425" yWindow="0" windowWidth="17280" windowHeight="8640" activeTab="1"/>
+    <workbookView xWindow="25350" yWindow="0" windowWidth="17280" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="88">
   <si>
     <t>Parameter</t>
   </si>
@@ -202,15 +202,6 @@
     <t>Rate for voltage cut-off in Open Mode (controller frequency dependent)</t>
   </si>
   <si>
-    <t>Maximum allowed motor current (continuous)</t>
-  </si>
-  <si>
-    <t>Field weakening current map</t>
-  </si>
-  <si>
-    <t>Field weakening X Axis</t>
-  </si>
-  <si>
     <t>Maximum motor speed</t>
   </si>
   <si>
@@ -275,6 +266,30 @@
   </si>
   <si>
     <t>Motor speed Low for field weakening authorization</t>
+  </si>
+  <si>
+    <t>a_phaAdv_M1</t>
+  </si>
+  <si>
+    <t>r_phaAdv_XA</t>
+  </si>
+  <si>
+    <t>sfix16_En8</t>
+  </si>
+  <si>
+    <t>Phase advance angle (only for SIN control type)</t>
+  </si>
+  <si>
+    <t>Phase advance X Axis (only for SIN control type)</t>
+  </si>
+  <si>
+    <t>Maximum allowed motor current</t>
+  </si>
+  <si>
+    <t>Field weakening X Axis (only for FOC control type)</t>
+  </si>
+  <si>
+    <t>Field weakening current map (only for FOC control type)</t>
   </si>
 </sst>
 </file>
@@ -344,13 +359,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,8 +385,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:D38" totalsRowShown="0">
-  <autoFilter ref="B3:D38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:D40" totalsRowShown="0">
+  <autoFilter ref="B3:D40"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Parameter"/>
     <tableColumn id="2" name="DataType"/>
@@ -643,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,15 +705,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -705,7 +721,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -713,15 +729,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -729,23 +745,23 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -753,71 +769,71 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
@@ -825,15 +841,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -841,7 +857,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -849,7 +865,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -857,7 +873,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -865,7 +881,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -873,7 +889,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -881,7 +897,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -889,15 +905,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -905,41 +921,57 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>38</v>
       </c>
     </row>
@@ -950,10 +982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D38"/>
+  <dimension ref="B3:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,354 +1043,376 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>61</v>
+      <c r="D30" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
         <v>24</v>
       </c>
-      <c r="D31" t="s">
-        <v>62</v>
+      <c r="D31" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>38</v>
       </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" t="s">
-        <v>64</v>
+      <c r="B34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>65</v>
+        <v>24</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
-        <v>67</v>
+      <c r="D40" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>